<commit_message>
Render uyumlu: Excel ve Google Drive hataları giderildi
</commit_message>
<xml_diff>
--- a/backend/OneDrive_lojistik.xlsx
+++ b/backend/OneDrive_lojistik.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,61 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>31.03.2026</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>9</v>
+      </c>
+      <c r="M3" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tam sürüm: Excel, OneDrive ve Google Drive uyumlu
</commit_message>
<xml_diff>
--- a/backend/OneDrive_lojistik.xlsx
+++ b/backend/OneDrive_lojistik.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,6 +598,61 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>31.03.2026</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>14</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Yeni çalışan proje - Google Drive ve Download eklendi
</commit_message>
<xml_diff>
--- a/backend/OneDrive_lojistik.xlsx
+++ b/backend/OneDrive_lojistik.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1093,6 +1093,116 @@
         <v>689</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>15.02.2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>68HS574</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>14</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Melih Karaman</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>9</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>11.07.2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>45HD132</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>564</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>614</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>617</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ela karaman </t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>116</v>
+      </c>
+      <c r="M14" t="n">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>